<commit_message>
adding open source drawings to breakout board projects
updating pinout on 14pin breakout + regenerating output files
</commit_message>
<xml_diff>
--- a/ee/Altium/Breakout_14pin/Project Outputs for Breakout_14pin/Breakout_14pin-RevA_PCBA_Files/BOM/Bill of Materials-Breakout_14pin(Mfg).xlsx
+++ b/ee/Altium/Breakout_14pin/Project Outputs for Breakout_14pin/Breakout_14pin-RevA_PCBA_Files/BOM/Bill of Materials-Breakout_14pin(Mfg).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jocap\OneDrive\Documents\GitHub\intercreate-designs\ee\Altium\Breakout_14pin\Project Outputs for Breakout_14pin\Breakout_14pin-RevA_PCBA_Files\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{27B571BB-3867-470C-AE63-DC72634D4617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8EABCF29-E8B1-4753-8699-8AFD9D911F26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3465" windowWidth="28770" windowHeight="13635" xr2:uid="{5202166A-FC30-42A1-9FEA-FD3BFC3C0F64}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="28800" windowHeight="17145" xr2:uid="{A84CBB20-511A-47EF-9F9A-9DC0D6368EDB}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-Breakout_14pi" sheetId="1" r:id="rId1"/>
@@ -451,7 +451,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FD47CF2-9774-48EE-BF16-0F9F3B9AD3E8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD658D94-4FAC-4752-8D92-8984B1B42826}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>